<commit_message>
modifikasi usulan pi, outline pi, dan ppt pi h-1 presentasi
</commit_message>
<xml_diff>
--- a/REFERENSI PI.xlsx
+++ b/REFERENSI PI.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alief\Documents\BERKAS PI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359BB0CC-4F89-4605-84E6-25F3949B270B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9678C56D-D4FB-4DA8-A24A-7C02932EDADF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1830" windowWidth="20730" windowHeight="11310" xr2:uid="{6ABDDA2A-3E43-4F2F-8896-9FC65328CABE}"/>
+    <workbookView xWindow="756" yWindow="1200" windowWidth="17280" windowHeight="9072" xr2:uid="{6ABDDA2A-3E43-4F2F-8896-9FC65328CABE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>NO</t>
   </si>
@@ -78,6 +79,9 @@
   </si>
   <si>
     <t>HASIL</t>
+  </si>
+  <si>
+    <t>DIAKSES TANGGAL</t>
   </si>
 </sst>
 </file>
@@ -459,31 +463,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{312ED076-8517-457C-B82B-F429C86284A9}">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="56.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -529,8 +534,11 @@
       <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -546,8 +554,9 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -563,8 +572,9 @@
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -580,8 +590,9 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -597,8 +608,9 @@
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P5" s="3"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -614,8 +626,9 @@
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -631,8 +644,9 @@
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -648,8 +662,9 @@
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P8" s="3"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -665,8 +680,9 @@
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -682,8 +698,9 @@
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P10" s="3"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -699,8 +716,9 @@
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P11" s="3"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -716,8 +734,9 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P12" s="3"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -733,8 +752,9 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P13" s="3"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -750,6 +770,7 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Memodifikasi file h+ bimbingan ke tiga
</commit_message>
<xml_diff>
--- a/REFERENSI PI.xlsx
+++ b/REFERENSI PI.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alief\Documents\BERKAS PI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9678C56D-D4FB-4DA8-A24A-7C02932EDADF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8837CC2-AE09-451A-964C-20DC0C637A07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="756" yWindow="1200" windowWidth="17280" windowHeight="9072" xr2:uid="{6ABDDA2A-3E43-4F2F-8896-9FC65328CABE}"/>
+    <workbookView xWindow="28680" yWindow="1830" windowWidth="20730" windowHeight="11310" xr2:uid="{6ABDDA2A-3E43-4F2F-8896-9FC65328CABE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>NO</t>
   </si>
@@ -82,6 +81,105 @@
   </si>
   <si>
     <t>DIAKSES TANGGAL</t>
+  </si>
+  <si>
+    <t>Kishore Baktha</t>
+  </si>
+  <si>
+    <t>Mobile Application Development: All the Steps and Guidelines for Successful Creation of Mobile App: Case Study</t>
+  </si>
+  <si>
+    <t>A Monthly Journal of Computer Science and Information Technology</t>
+  </si>
+  <si>
+    <t>International Journal of Computer Science and Mobile Computing</t>
+  </si>
+  <si>
+    <t>15-20</t>
+  </si>
+  <si>
+    <t>Research and Development of Mobile Application for Android Platform</t>
+  </si>
+  <si>
+    <t>Li Ma1,2,3 , Lei Gu1,2 and Jin Wang1,2,3</t>
+  </si>
+  <si>
+    <t>International Journal of Multimedia and Ubiquitous Engineering</t>
+  </si>
+  <si>
+    <t>FACTORS INFLUENCING QUALITY OF MOBILE APPS: ROLE OF MOBILE APP DEVELOPMENT LIFE CYCLE</t>
+  </si>
+  <si>
+    <t>International Journal of Software Engineering &amp; Applications</t>
+  </si>
+  <si>
+    <t>Venkata N Inukollu1 , Divya D Keshamoni2 , Taeghyun Kang 3 and Manikanta Inukollu4</t>
+  </si>
+  <si>
+    <t>Research on Development of Android Applications</t>
+  </si>
+  <si>
+    <t>IOSR Journal of Computer Engineering</t>
+  </si>
+  <si>
+    <t>28-32</t>
+  </si>
+  <si>
+    <t>Review Study on New Era of Android Kotlin</t>
+  </si>
+  <si>
+    <t>Mrs. Prachi Sasankar1 . Mrs. Usha Kosarkar. 2</t>
+  </si>
+  <si>
+    <t>1Jahanvee Narang, 2Er.Salony Tuli</t>
+  </si>
+  <si>
+    <t>INTERNATIONAL JOURNAL OF TECHNOLOGY AND COMPUTING (IJTC)</t>
+  </si>
+  <si>
+    <t>271-273</t>
+  </si>
+  <si>
+    <t>KOTLIN - A New Programming Language for the Modern Needs</t>
+  </si>
+  <si>
+    <t>[1] Mrs.J.ArockiaJeyanthi, [2] Mrs.T.Kamaleswari</t>
+  </si>
+  <si>
+    <t>International Journal of Science, Engineering and Management (IJSEM)</t>
+  </si>
+  <si>
+    <t>271-275</t>
+  </si>
+  <si>
+    <t>Model of E-Volunteer : A Preliminary Study to Develop Application to Support Volunteering Activities in Indonesia</t>
+  </si>
+  <si>
+    <t>Anita Ratnasari1, Wachyu Hari Haji 2</t>
+  </si>
+  <si>
+    <t>305-310</t>
+  </si>
+  <si>
+    <t>Rahmatsyah1 , Agi Putra Kharisma2 , Sutrisno</t>
+  </si>
+  <si>
+    <t>Pengembangan Aplikasi Perangkat Bergerak Layanan berbasis Lokasi Penghubung Sukarelawan dengan Kegiatan Sukarela</t>
+  </si>
+  <si>
+    <t>Jurnal Pengembangan Teknologi Informasi dan Ilmu Komputer</t>
+  </si>
+  <si>
+    <t>9859-9866</t>
+  </si>
+  <si>
+    <t>VOLUNTEER BENERAN INDONESIA: KETERLIBATAN DAN KOMITMEN WARGA NEGARA MUDA DI DALAM KOMUNITAS BERLATARBELAKANG MULTIKULTUR</t>
+  </si>
+  <si>
+    <t>Muhammad Mona Adha, Eska Prawisudawati Ulpa, Dasim Budimansyah, Jack McGregor Johnstone</t>
+  </si>
+  <si>
+    <t>JIPPK</t>
   </si>
 </sst>
 </file>
@@ -144,11 +242,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,22 +569,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{312ED076-8517-457C-B82B-F429C86284A9}">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="125.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="56.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="78.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="57.77734375" customWidth="1"/>
+    <col min="10" max="10" width="107.33203125" customWidth="1"/>
+    <col min="11" max="11" width="82.88671875" customWidth="1"/>
     <col min="12" max="12" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="25" bestFit="1" customWidth="1"/>
@@ -538,18 +642,34 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2017</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="3">
+        <v>6</v>
+      </c>
+      <c r="G2" s="3">
+        <v>9</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="5"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -558,13 +678,25 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2014</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
       <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="F3" s="3">
+        <v>9</v>
+      </c>
+      <c r="G3" s="3">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -574,15 +706,27 @@
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="B4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2014</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
       <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="F4" s="3">
+        <v>5</v>
+      </c>
+      <c r="G4" s="3">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -594,14 +738,24 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2016</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
@@ -612,14 +766,24 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2017</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="H6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
@@ -630,14 +794,28 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2017</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+      <c r="F7" s="3">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -648,14 +826,26 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2018</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="3">
+        <v>3</v>
+      </c>
+      <c r="G8" s="3">
+        <v>6</v>
+      </c>
       <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="I8" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -666,14 +856,28 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2019</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
       <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="F9" s="3">
+        <v>3</v>
+      </c>
+      <c r="G9" s="3">
+        <v>10</v>
+      </c>
+      <c r="H9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
@@ -682,15 +886,25 @@
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
+      <c r="B10" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="D10" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="F10" s="3">
+        <v>4</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>48</v>
+      </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>

</xml_diff>